<commit_message>
updates associated with new reoworking of draft manuscript.the new_plots.R script is new controlling scrift for simulation and figure generation.
</commit_message>
<xml_diff>
--- a/data/broodstock_remova.xlsx
+++ b/data/broodstock_remova.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwnetid-my.sharepoint.com/personal/marks6_uw_edu/Documents/Documents/Wenatchee/Wenatchee-IPM/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/mark_sorel_dfw_wa_gov/Documents/Documents/Sorel_etal_mgmt_modeling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="8_{484FE93A-B490-4CFA-A570-BEDABA6ABE3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E95C752-0C17-4FAE-9549-0126555F364D}"/>
+  <xr:revisionPtr revIDLastSave="150" documentId="8_{484FE93A-B490-4CFA-A570-BEDABA6ABE3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{657866E4-008A-4990-86BB-B0F4B6B27749}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{3ED6D4EC-3CCF-4159-BBB7-230377ED695C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{3ED6D4EC-3CCF-4159-BBB7-230377ED695C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet2!#REF!</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="21">
   <si>
     <t>Brood_year</t>
   </si>
@@ -99,6 +96,9 @@
   <si>
     <t>smolts_released</t>
   </si>
+  <si>
+    <t>Stream</t>
+  </si>
 </sst>
 </file>
 
@@ -133,9 +133,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -154,9 +155,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -194,7 +195,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -300,7 +301,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -442,7 +443,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -453,12 +454,12 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -481,7 +482,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1989</v>
       </c>
@@ -495,7 +496,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1990</v>
       </c>
@@ -509,7 +510,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1991</v>
       </c>
@@ -532,7 +533,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1992</v>
       </c>
@@ -555,7 +556,7 @@
         <v>0.71399999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1993</v>
       </c>
@@ -578,7 +579,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1994</v>
       </c>
@@ -601,7 +602,7 @@
         <v>0.71399999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1995</v>
       </c>
@@ -624,7 +625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1996</v>
       </c>
@@ -647,7 +648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1997</v>
       </c>
@@ -670,7 +671,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1998</v>
       </c>
@@ -693,7 +694,7 @@
         <v>0.36399999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1999</v>
       </c>
@@ -716,7 +717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2000</v>
       </c>
@@ -739,7 +740,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2001</v>
       </c>
@@ -762,7 +763,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2002</v>
       </c>
@@ -785,7 +786,7 @@
         <v>0.33300000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2003</v>
       </c>
@@ -808,7 +809,7 @@
         <v>0.70299999999999996</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2004</v>
       </c>
@@ -831,7 +832,7 @@
         <v>4.1000000000000002E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2005</v>
       </c>
@@ -854,7 +855,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2006</v>
       </c>
@@ -877,7 +878,7 @@
         <v>0.27600000000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2007</v>
       </c>
@@ -900,7 +901,7 @@
         <v>0.311</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2008</v>
       </c>
@@ -923,7 +924,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2009</v>
       </c>
@@ -946,7 +947,7 @@
         <v>0.124</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2010</v>
       </c>
@@ -969,7 +970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2011</v>
       </c>
@@ -992,7 +993,7 @@
         <v>0.44600000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2012</v>
       </c>
@@ -1015,7 +1016,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2013</v>
       </c>
@@ -1038,7 +1039,7 @@
         <v>0.34300000000000003</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2014</v>
       </c>
@@ -1061,7 +1062,7 @@
         <v>8.7999999999999995E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2015</v>
       </c>
@@ -1084,7 +1085,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2016</v>
       </c>
@@ -1107,7 +1108,7 @@
         <v>0.17399999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2017</v>
       </c>
@@ -1130,7 +1131,7 @@
         <v>8.5000000000000006E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>2018</v>
       </c>
@@ -1153,7 +1154,7 @@
         <v>0.16700000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>2019</v>
       </c>
@@ -1183,15 +1184,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C5C8740-EEE7-4BD0-BA69-71C7C4C336AC}">
-  <dimension ref="A1:L62"/>
+  <dimension ref="A1:L68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1222,8 +1223,11 @@
       <c r="J1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1254,9 +1258,11 @@
       <c r="J2" s="1">
         <v>85113</v>
       </c>
-      <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1287,9 +1293,11 @@
       <c r="J3" s="1">
         <v>223610</v>
       </c>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1320,9 +1328,11 @@
       <c r="J4" s="1">
         <v>27226</v>
       </c>
-      <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1350,8 +1360,11 @@
       <c r="I5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1382,9 +1395,11 @@
       <c r="J6" s="1">
         <v>15176</v>
       </c>
-      <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1415,9 +1430,11 @@
       <c r="J7" s="1">
         <v>266148</v>
       </c>
-      <c r="K7" s="1"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1448,9 +1465,11 @@
       <c r="J8" s="1">
         <v>75906</v>
       </c>
-      <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K8" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1478,8 +1497,11 @@
       <c r="I9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1510,9 +1532,11 @@
       <c r="J10" s="1">
         <v>47104</v>
       </c>
-      <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1541,8 +1565,11 @@
         <v>0.32</v>
       </c>
       <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K11" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1573,8 +1600,11 @@
       <c r="J12" s="1">
         <v>149668</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K12" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1605,8 +1635,11 @@
       <c r="J13" s="1">
         <v>222131</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K13" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1637,8 +1670,11 @@
       <c r="J14" s="1">
         <v>494517</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K14" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1669,9 +1705,11 @@
       <c r="J15" s="1">
         <v>494012</v>
       </c>
-      <c r="K15" s="1"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K15" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1702,8 +1740,11 @@
       <c r="J16" s="1">
         <v>612482</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K16" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1734,8 +1775,11 @@
       <c r="J17" s="1">
         <v>305542</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K17" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1766,8 +1810,11 @@
       <c r="J18" s="1">
         <v>609789</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K18" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -1798,8 +1845,11 @@
       <c r="J19" s="1">
         <v>438561</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K19" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -1830,8 +1880,11 @@
       <c r="J20" s="1">
         <v>346248</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K20" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -1862,8 +1915,11 @@
       <c r="J21" s="1">
         <v>281821</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K21" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -1894,8 +1950,11 @@
       <c r="J22" s="1">
         <v>222504</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K22" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -1926,8 +1985,11 @@
       <c r="J23" s="1">
         <v>147480</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K23" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -1956,8 +2018,11 @@
         <v>0.65</v>
       </c>
       <c r="J24" s="1"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K24" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -1988,8 +2053,11 @@
       <c r="J25" s="1">
         <v>163411</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K25" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -2020,8 +2088,11 @@
       <c r="J26" s="1">
         <v>158189</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K26" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -2052,8 +2123,11 @@
       <c r="J27" s="1">
         <v>149867</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K27" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -2084,8 +2158,11 @@
       <c r="J28" s="1">
         <v>165888</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K28" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -2113,8 +2190,11 @@
       <c r="I29">
         <v>0.42</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K29" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -2142,107 +2222,103 @@
       <c r="I30">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>18</v>
-      </c>
+      <c r="K30" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B31">
+        <v>2021</v>
+      </c>
+      <c r="C31">
+        <v>310</v>
+      </c>
+      <c r="D31">
+        <v>330</v>
+      </c>
+      <c r="E31" s="2">
+        <f>D31/(D31+C31)</f>
+        <v>0.515625</v>
+      </c>
+      <c r="F31">
+        <v>73</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31" s="2">
+        <f>F31/(G31+F31)</f>
+        <v>1</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>2022</v>
+      </c>
+      <c r="C32">
+        <v>424</v>
+      </c>
+      <c r="D32">
+        <v>476</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" ref="E32:E33" si="0">D32/(D32+C32)</f>
+        <v>0.52888888888888885</v>
+      </c>
+      <c r="F32">
+        <v>72</v>
+      </c>
+      <c r="G32">
+        <v>7</v>
+      </c>
+      <c r="H32" s="2">
+        <f t="shared" ref="H32:H33" si="1">F32/(G32+F32)</f>
+        <v>0.91139240506329111</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>2023</v>
+      </c>
+      <c r="C33">
+        <v>348</v>
+      </c>
+      <c r="D33">
+        <v>123</v>
+      </c>
+      <c r="E33" s="2">
+        <f t="shared" si="0"/>
+        <v>0.26114649681528662</v>
+      </c>
+      <c r="F33">
+        <v>77</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34">
         <v>1989</v>
       </c>
-      <c r="C31">
+      <c r="C34">
         <v>288</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
-      <c r="H31">
-        <v>1</v>
-      </c>
-      <c r="I31">
-        <v>1</v>
-      </c>
-      <c r="K31" s="1"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>18</v>
-      </c>
-      <c r="B32">
-        <v>1990</v>
-      </c>
-      <c r="C32">
-        <v>235</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="H32">
-        <v>1</v>
-      </c>
-      <c r="I32">
-        <v>1</v>
-      </c>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>18</v>
-      </c>
-      <c r="B33">
-        <v>1991</v>
-      </c>
-      <c r="C33">
-        <v>156</v>
-      </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
-      <c r="H33">
-        <v>1</v>
-      </c>
-      <c r="I33">
-        <v>1</v>
-      </c>
-      <c r="K33" s="1"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>18</v>
-      </c>
-      <c r="B34">
-        <v>1992</v>
-      </c>
-      <c r="C34">
-        <v>181</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -2262,23 +2338,25 @@
       <c r="I34">
         <v>1</v>
       </c>
-      <c r="K34" s="1"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K34" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>18</v>
       </c>
       <c r="B35">
-        <v>1993</v>
+        <v>1990</v>
       </c>
       <c r="C35">
-        <v>430</v>
+        <v>235</v>
       </c>
       <c r="D35">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="E35">
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -2290,18 +2368,22 @@
         <v>1</v>
       </c>
       <c r="I35">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L35" s="1"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>18</v>
       </c>
       <c r="B36">
-        <v>1994</v>
+        <v>1991</v>
       </c>
       <c r="C36">
-        <v>60</v>
+        <v>156</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -2316,22 +2398,24 @@
         <v>0</v>
       </c>
       <c r="H36">
-        <v>0.67</v>
+        <v>1</v>
       </c>
       <c r="I36">
         <v>1</v>
       </c>
-      <c r="K36" s="1"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K36" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>18</v>
       </c>
       <c r="B37">
-        <v>1995</v>
+        <v>1992</v>
       </c>
       <c r="C37">
-        <v>18</v>
+        <v>181</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -2346,748 +2430,1005 @@
         <v>0</v>
       </c>
       <c r="H37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K37" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>18</v>
       </c>
       <c r="B38">
+        <v>1993</v>
+      </c>
+      <c r="C38">
+        <v>430</v>
+      </c>
+      <c r="D38">
+        <v>61</v>
+      </c>
+      <c r="E38">
+        <v>0.12</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38">
+        <v>0.9</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39">
+        <v>1994</v>
+      </c>
+      <c r="C39">
+        <v>60</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0.67</v>
+      </c>
+      <c r="I39">
+        <v>1</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40">
+        <v>1995</v>
+      </c>
+      <c r="C40">
+        <v>18</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>1</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41">
         <v>1996</v>
       </c>
-      <c r="C38">
+      <c r="C41">
         <v>58</v>
       </c>
-      <c r="D38">
+      <c r="D41">
         <v>25</v>
       </c>
-      <c r="E38">
+      <c r="E41">
         <v>0.3</v>
       </c>
-      <c r="F38">
-        <v>0</v>
-      </c>
-      <c r="G38">
-        <v>0</v>
-      </c>
-      <c r="H38">
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
         <v>0.44</v>
       </c>
-      <c r="I38">
+      <c r="I41">
         <v>0.61</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>18</v>
-      </c>
-      <c r="B39">
+      <c r="K41" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>18</v>
+      </c>
+      <c r="B42">
         <v>1997</v>
       </c>
-      <c r="C39">
+      <c r="C42">
         <v>67</v>
       </c>
-      <c r="D39">
+      <c r="D42">
         <v>55</v>
       </c>
-      <c r="E39">
+      <c r="E42">
         <v>0.45</v>
       </c>
-      <c r="F39">
-        <v>0</v>
-      </c>
-      <c r="G39">
-        <v>0</v>
-      </c>
-      <c r="H39">
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I39">
+      <c r="I42">
         <v>0.42</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>18</v>
-      </c>
-      <c r="B40">
+      <c r="K42" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43">
         <v>1998</v>
       </c>
-      <c r="C40">
+      <c r="C43">
         <v>61</v>
       </c>
-      <c r="D40">
+      <c r="D43">
         <v>3</v>
       </c>
-      <c r="E40">
+      <c r="E43">
         <v>0.05</v>
       </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-      <c r="G40">
-        <v>0</v>
-      </c>
-      <c r="H40">
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I40">
+      <c r="I43">
         <v>0.86</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>18</v>
-      </c>
-      <c r="B41">
+      <c r="K43" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44">
         <v>1999</v>
       </c>
-      <c r="C41">
+      <c r="C44">
         <v>22</v>
       </c>
-      <c r="D41">
-        <v>0</v>
-      </c>
-      <c r="E41">
-        <v>0</v>
-      </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-      <c r="G41">
-        <v>0</v>
-      </c>
-      <c r="H41">
-        <v>0</v>
-      </c>
-      <c r="I41">
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>18</v>
-      </c>
-      <c r="B42">
+      <c r="K44" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45">
         <v>2000</v>
       </c>
-      <c r="C42">
+      <c r="C45">
         <v>189</v>
       </c>
-      <c r="D42">
+      <c r="D45">
         <v>81</v>
       </c>
-      <c r="E42">
+      <c r="E45">
         <v>0.3</v>
       </c>
-      <c r="F42">
-        <v>0</v>
-      </c>
-      <c r="G42">
-        <v>0</v>
-      </c>
-      <c r="H42">
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
         <v>0.3</v>
       </c>
-      <c r="I42">
+      <c r="I45">
         <v>0.52</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>18</v>
-      </c>
-      <c r="B43">
+      <c r="K45" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46">
         <v>2001</v>
       </c>
-      <c r="C43">
+      <c r="C46">
         <v>257</v>
       </c>
-      <c r="D43">
+      <c r="D46">
         <v>341</v>
       </c>
-      <c r="E43">
+      <c r="E46">
         <v>0.56999999999999995</v>
       </c>
-      <c r="F43">
-        <v>0</v>
-      </c>
-      <c r="G43">
-        <v>0</v>
-      </c>
-      <c r="H43">
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
         <v>0.3</v>
       </c>
-      <c r="I43">
+      <c r="I46">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>18</v>
-      </c>
-      <c r="B44">
+      <c r="K46" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>18</v>
+      </c>
+      <c r="B47">
         <v>2002</v>
       </c>
-      <c r="C44">
+      <c r="C47">
         <v>313</v>
       </c>
-      <c r="D44">
+      <c r="D47">
         <v>290</v>
       </c>
-      <c r="E44">
+      <c r="E47">
         <v>0.48</v>
       </c>
-      <c r="F44">
-        <v>0</v>
-      </c>
-      <c r="G44">
-        <v>0</v>
-      </c>
-      <c r="H44">
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I44">
+      <c r="I47">
         <v>0.39</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>18</v>
-      </c>
-      <c r="B45">
+      <c r="K47" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48">
         <v>2003</v>
       </c>
-      <c r="C45">
+      <c r="C48">
         <v>152</v>
       </c>
-      <c r="D45">
+      <c r="D48">
         <v>50</v>
       </c>
-      <c r="E45">
+      <c r="E48">
         <v>0.25</v>
       </c>
-      <c r="F45">
-        <v>0</v>
-      </c>
-      <c r="G45">
-        <v>0</v>
-      </c>
-      <c r="H45">
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
         <v>0.44</v>
       </c>
-      <c r="I45">
+      <c r="I48">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>18</v>
-      </c>
-      <c r="B46">
+      <c r="K48" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>18</v>
+      </c>
+      <c r="B49">
         <v>2004</v>
       </c>
-      <c r="C46">
+      <c r="C49">
         <v>297</v>
       </c>
-      <c r="D46">
+      <c r="D49">
         <v>210</v>
       </c>
-      <c r="E46">
+      <c r="E49">
         <v>0.41</v>
       </c>
-      <c r="F46">
-        <v>0</v>
-      </c>
-      <c r="G46">
-        <v>0</v>
-      </c>
-      <c r="H46">
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
         <v>0.39</v>
       </c>
-      <c r="I46">
+      <c r="I49">
         <v>0.51</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>18</v>
-      </c>
-      <c r="B47">
+      <c r="K49" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>18</v>
+      </c>
+      <c r="B50">
         <v>2005</v>
       </c>
-      <c r="C47">
+      <c r="C50">
         <v>81</v>
       </c>
-      <c r="D47">
+      <c r="D50">
         <v>266</v>
       </c>
-      <c r="E47">
+      <c r="E50">
         <v>0.77</v>
       </c>
-      <c r="F47">
-        <v>0</v>
-      </c>
-      <c r="G47">
-        <v>0</v>
-      </c>
-      <c r="H47">
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
         <v>0.33</v>
       </c>
-      <c r="I47">
+      <c r="I50">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>18</v>
-      </c>
-      <c r="B48">
+      <c r="K50" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>18</v>
+      </c>
+      <c r="B51">
         <v>2006</v>
       </c>
-      <c r="C48">
+      <c r="C51">
         <v>117</v>
       </c>
-      <c r="D48">
+      <c r="D51">
         <v>154</v>
       </c>
-      <c r="E48">
+      <c r="E51">
         <v>0.56999999999999995</v>
       </c>
-      <c r="F48">
-        <v>0</v>
-      </c>
-      <c r="G48">
-        <v>0</v>
-      </c>
-      <c r="H48">
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I48">
+      <c r="I51">
         <v>0.36</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>18</v>
-      </c>
-      <c r="B49">
+      <c r="K51" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>18</v>
+      </c>
+      <c r="B52">
         <v>2007</v>
       </c>
-      <c r="C49">
+      <c r="C52">
         <v>83</v>
       </c>
-      <c r="D49">
+      <c r="D52">
         <v>380</v>
       </c>
-      <c r="E49">
+      <c r="E52">
         <v>0.82</v>
       </c>
-      <c r="F49">
-        <v>0</v>
-      </c>
-      <c r="G49">
-        <v>0</v>
-      </c>
-      <c r="H49">
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I49">
+      <c r="I52">
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>18</v>
-      </c>
-      <c r="B50">
+      <c r="K52" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>18</v>
+      </c>
+      <c r="B53">
         <v>2008</v>
       </c>
-      <c r="C50">
+      <c r="C53">
         <v>139</v>
       </c>
-      <c r="D50">
+      <c r="D53">
         <v>425</v>
       </c>
-      <c r="E50">
+      <c r="E53">
         <v>0.75</v>
       </c>
-      <c r="F50">
-        <v>0</v>
-      </c>
-      <c r="G50">
-        <v>0</v>
-      </c>
-      <c r="H50">
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
         <v>0.27</v>
       </c>
-      <c r="I50">
+      <c r="I53">
         <v>0.28999999999999998</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>18</v>
-      </c>
-      <c r="B51">
+      <c r="K53" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>18</v>
+      </c>
+      <c r="B54">
         <v>2009</v>
       </c>
-      <c r="C51">
+      <c r="C54">
         <v>163</v>
       </c>
-      <c r="D51">
+      <c r="D54">
         <v>371</v>
       </c>
-      <c r="E51">
+      <c r="E54">
         <v>0.69</v>
       </c>
-      <c r="F51">
-        <v>0</v>
-      </c>
-      <c r="G51">
-        <v>0</v>
-      </c>
-      <c r="H51">
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
         <v>0.46</v>
       </c>
-      <c r="I51">
+      <c r="I54">
         <v>0.42</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>18</v>
-      </c>
-      <c r="B52">
+      <c r="K54" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>18</v>
+      </c>
+      <c r="B55">
         <v>2010</v>
       </c>
-      <c r="C52">
+      <c r="C55">
         <v>59</v>
       </c>
-      <c r="D52">
+      <c r="D55">
         <v>349</v>
       </c>
-      <c r="E52">
+      <c r="E55">
         <v>0.86</v>
       </c>
-      <c r="F52">
-        <v>0</v>
-      </c>
-      <c r="G52">
-        <v>0</v>
-      </c>
-      <c r="H52">
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
         <v>0.44</v>
       </c>
-      <c r="I52">
+      <c r="I55">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>18</v>
-      </c>
-      <c r="B53">
+      <c r="K55" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>18</v>
+      </c>
+      <c r="B56">
         <v>2011</v>
       </c>
-      <c r="C53">
+      <c r="C56">
         <v>250</v>
       </c>
-      <c r="D53">
+      <c r="D56">
         <v>452</v>
       </c>
-      <c r="E53">
+      <c r="E56">
         <v>0.64</v>
       </c>
-      <c r="F53">
-        <v>0</v>
-      </c>
-      <c r="G53">
-        <v>0</v>
-      </c>
-      <c r="H53">
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
         <v>0.46</v>
       </c>
-      <c r="I53">
+      <c r="I56">
         <v>0.43</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>18</v>
-      </c>
-      <c r="B54">
+      <c r="K56" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>18</v>
+      </c>
+      <c r="B57">
         <v>2012</v>
       </c>
-      <c r="C54">
+      <c r="C57">
         <v>220</v>
       </c>
-      <c r="D54">
+      <c r="D57">
         <v>474</v>
       </c>
-      <c r="E54">
+      <c r="E57">
         <v>0.68</v>
       </c>
-      <c r="F54">
-        <v>0</v>
-      </c>
-      <c r="G54">
-        <v>0</v>
-      </c>
-      <c r="H54">
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
         <v>0.66</v>
       </c>
-      <c r="I54">
+      <c r="I57">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>18</v>
-      </c>
-      <c r="B55">
+      <c r="K57" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>18</v>
+      </c>
+      <c r="B58">
         <v>2013</v>
       </c>
-      <c r="C55">
+      <c r="C58">
         <v>70</v>
       </c>
-      <c r="D55">
+      <c r="D58">
         <v>339</v>
       </c>
-      <c r="E55">
+      <c r="E58">
         <v>0.83</v>
       </c>
-      <c r="F55">
+      <c r="F58">
         <v>20</v>
       </c>
-      <c r="G55">
+      <c r="G58">
         <v>5</v>
       </c>
-      <c r="H55">
+      <c r="H58">
         <v>0.8</v>
       </c>
-      <c r="I55">
+      <c r="I58">
         <v>0.5</v>
       </c>
-      <c r="J55" s="1">
+      <c r="J58" s="1">
         <v>43082</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>18</v>
-      </c>
-      <c r="B56">
+      <c r="K58" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>18</v>
+      </c>
+      <c r="B59">
         <v>2014</v>
       </c>
-      <c r="C56">
+      <c r="C59">
         <v>165</v>
       </c>
-      <c r="D56">
+      <c r="D59">
         <v>66</v>
       </c>
-      <c r="E56">
+      <c r="E59">
         <v>0.28999999999999998</v>
       </c>
-      <c r="F56">
+      <c r="F59">
         <v>21</v>
       </c>
-      <c r="G56">
-        <v>0</v>
-      </c>
-      <c r="H56">
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59">
         <v>1</v>
       </c>
-      <c r="I56">
+      <c r="I59">
         <v>0.78</v>
       </c>
-      <c r="J56" s="1"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>18</v>
-      </c>
-      <c r="B57">
+      <c r="J59" s="1"/>
+      <c r="K59" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>18</v>
+      </c>
+      <c r="B60">
         <v>2015</v>
       </c>
-      <c r="C57">
+      <c r="C60">
         <v>130</v>
       </c>
-      <c r="D57">
+      <c r="D60">
         <v>21</v>
       </c>
-      <c r="E57">
+      <c r="E60">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F57">
+      <c r="F60">
         <v>60</v>
       </c>
-      <c r="G57">
+      <c r="G60">
         <v>63</v>
       </c>
-      <c r="H57">
+      <c r="H60">
         <v>0.49</v>
       </c>
-      <c r="I57">
+      <c r="I60">
         <v>0.79</v>
       </c>
-      <c r="J57" s="1">
+      <c r="J60" s="1">
         <v>243127</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>18</v>
-      </c>
-      <c r="B58">
+      <c r="K60" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>18</v>
+      </c>
+      <c r="B61">
         <v>2016</v>
       </c>
-      <c r="C58">
+      <c r="C61">
         <v>120</v>
       </c>
-      <c r="D58">
+      <c r="D61">
         <v>29</v>
       </c>
-      <c r="E58">
+      <c r="E61">
         <v>0.26</v>
       </c>
-      <c r="F58">
+      <c r="F61">
         <v>70</v>
       </c>
-      <c r="G58">
+      <c r="G61">
         <v>66</v>
       </c>
-      <c r="H58">
+      <c r="H61">
         <v>0.51</v>
       </c>
-      <c r="I58">
+      <c r="I61">
         <v>0.74</v>
       </c>
-      <c r="J58" s="1">
+      <c r="J61" s="1">
         <v>233471</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>18</v>
-      </c>
-      <c r="B59">
+      <c r="K61" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>18</v>
+      </c>
+      <c r="B62">
         <v>2017</v>
       </c>
-      <c r="C59">
+      <c r="C62">
         <v>61</v>
       </c>
-      <c r="D59">
+      <c r="D62">
         <v>71</v>
       </c>
-      <c r="E59">
+      <c r="E62">
         <v>0.78</v>
       </c>
-      <c r="F59">
+      <c r="F62">
         <v>70</v>
       </c>
-      <c r="G59">
+      <c r="G62">
         <v>64</v>
       </c>
-      <c r="H59">
+      <c r="H62">
         <v>0.52</v>
       </c>
-      <c r="I59">
+      <c r="I62">
         <v>0.51</v>
       </c>
-      <c r="J59" s="1">
+      <c r="J62" s="1">
         <v>231859</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>18</v>
-      </c>
-      <c r="B60">
+      <c r="K62" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>18</v>
+      </c>
+      <c r="B63">
         <v>2018</v>
       </c>
-      <c r="C60">
+      <c r="C63">
         <v>21</v>
       </c>
-      <c r="D60">
+      <c r="D63">
         <v>148</v>
       </c>
-      <c r="E60">
+      <c r="E63">
         <v>1.29</v>
       </c>
-      <c r="F60">
+      <c r="F63">
         <v>53</v>
       </c>
-      <c r="G60">
+      <c r="G63">
         <v>54</v>
       </c>
-      <c r="H60">
+      <c r="H63">
         <v>0.5</v>
       </c>
-      <c r="I60">
+      <c r="I63">
         <v>0.38</v>
       </c>
-      <c r="J60" s="1">
+      <c r="J63" s="1">
         <v>206508</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>18</v>
-      </c>
-      <c r="B61">
+      <c r="K63" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>18</v>
+      </c>
+      <c r="B64">
         <v>2019</v>
       </c>
-      <c r="C61">
+      <c r="C64">
         <v>35</v>
       </c>
-      <c r="D61">
+      <c r="D64">
         <v>345</v>
       </c>
-      <c r="E61">
+      <c r="E64">
         <v>1.77</v>
       </c>
-      <c r="F61">
+      <c r="F64">
         <v>47</v>
       </c>
-      <c r="G61">
+      <c r="G64">
         <v>85</v>
       </c>
-      <c r="H61">
+      <c r="H64">
         <v>0.36</v>
       </c>
-      <c r="I61">
+      <c r="I64">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>18</v>
-      </c>
-      <c r="B62">
+      <c r="K64" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>18</v>
+      </c>
+      <c r="B65">
         <v>2020</v>
       </c>
-      <c r="C62">
+      <c r="C65">
         <v>89</v>
       </c>
-      <c r="E62">
+      <c r="D65">
+        <v>280</v>
+      </c>
+      <c r="E65">
         <v>0.76</v>
       </c>
-      <c r="F62">
+      <c r="F65">
         <v>55</v>
       </c>
-      <c r="G62">
+      <c r="G65">
         <v>61</v>
       </c>
-      <c r="H62">
+      <c r="H65">
         <v>0.47</v>
       </c>
-      <c r="I62">
+      <c r="I65">
         <v>0.31</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B66">
+        <v>2021</v>
+      </c>
+      <c r="C66">
+        <v>122</v>
+      </c>
+      <c r="D66">
+        <f>455+74</f>
+        <v>529</v>
+      </c>
+      <c r="E66" s="2">
+        <f>D66/(D66+C66)</f>
+        <v>0.8125960061443932</v>
+      </c>
+      <c r="F66">
+        <v>64</v>
+      </c>
+      <c r="G66">
+        <v>61</v>
+      </c>
+      <c r="H66" s="2">
+        <f>F66/(G66+F66)</f>
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B67">
+        <v>2022</v>
+      </c>
+      <c r="C67">
+        <v>177</v>
+      </c>
+      <c r="D67">
+        <f>574+139</f>
+        <v>713</v>
+      </c>
+      <c r="E67" s="2">
+        <f t="shared" ref="E67:E68" si="2">D67/(D67+C67)</f>
+        <v>0.80112359550561796</v>
+      </c>
+      <c r="F67">
+        <v>65</v>
+      </c>
+      <c r="G67">
+        <v>54</v>
+      </c>
+      <c r="H67" s="2">
+        <f t="shared" ref="H67:H68" si="3">F67/(G67+F67)</f>
+        <v>0.54621848739495793</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B68">
+        <v>2023</v>
+      </c>
+      <c r="C68">
+        <v>110</v>
+      </c>
+      <c r="E68" s="2"/>
+      <c r="F68">
+        <v>69</v>
+      </c>
+      <c r="G68">
+        <v>51</v>
+      </c>
+      <c r="H68" s="2">
+        <f t="shared" si="3"/>
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>